<commit_message>
Added bfs to scan all rooms and assign lobbies
</commit_message>
<xml_diff>
--- a/building_test.xlsx
+++ b/building_test.xlsx
@@ -11,7 +11,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+  <si>
+    <t>Room  121</t>
+  </si>
+  <si>
+    <t>Room 122</t>
+  </si>
+  <si>
+    <t>Room  122</t>
+  </si>
+  <si>
+    <t>Room 123</t>
+  </si>
+  <si>
+    <t>Room  123</t>
+  </si>
+  <si>
+    <t>hall</t>
+  </si>
   <si>
     <t>Room 105</t>
   </si>
@@ -28,7 +46,19 @@
     <t>Room 101</t>
   </si>
   <si>
-    <t>hall</t>
+    <t>Room  128</t>
+  </si>
+  <si>
+    <t>Room 127</t>
+  </si>
+  <si>
+    <t>Room  126</t>
+  </si>
+  <si>
+    <t>Room 125</t>
+  </si>
+  <si>
+    <t>Room  124</t>
   </si>
   <si>
     <t>Room 106</t>
@@ -74,6 +104,66 @@
   </si>
   <si>
     <t>Room 120</t>
+  </si>
+  <si>
+    <t>Room 129</t>
+  </si>
+  <si>
+    <t>Room 148</t>
+  </si>
+  <si>
+    <t>Room 130</t>
+  </si>
+  <si>
+    <t>Room 147</t>
+  </si>
+  <si>
+    <t>Room 131</t>
+  </si>
+  <si>
+    <t>Room 146</t>
+  </si>
+  <si>
+    <t>Room 132</t>
+  </si>
+  <si>
+    <t>Room 145</t>
+  </si>
+  <si>
+    <t>Room 133</t>
+  </si>
+  <si>
+    <t>Room 144</t>
+  </si>
+  <si>
+    <t>Room 134</t>
+  </si>
+  <si>
+    <t>Room 143</t>
+  </si>
+  <si>
+    <t>Room 135</t>
+  </si>
+  <si>
+    <t>Room 142</t>
+  </si>
+  <si>
+    <t>Room 136</t>
+  </si>
+  <si>
+    <t>Room 141</t>
+  </si>
+  <si>
+    <t>Room 137</t>
+  </si>
+  <si>
+    <t>Room 140</t>
+  </si>
+  <si>
+    <t>Room 138</t>
+  </si>
+  <si>
+    <t>Room 139</t>
   </si>
 </sst>
 </file>
@@ -368,11 +458,6 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -396,11 +481,21 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -424,11 +519,21 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -447,26 +552,36 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -485,6 +600,18 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="1"/>
@@ -511,19 +638,19 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -577,19 +704,19 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -615,6 +742,18 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="1"/>
@@ -641,19 +780,19 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -711,9 +850,15 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="F13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -739,9 +884,15 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -767,9 +918,15 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="F15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -795,9 +952,15 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="F16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -823,9 +986,15 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="F17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -851,9 +1020,15 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="F18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -879,9 +1054,15 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="F19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -907,9 +1088,15 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="F20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -935,9 +1122,15 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="F21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -963,9 +1156,15 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="F22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -991,7 +1190,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="2"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1019,7 +1218,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1047,7 +1246,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="2"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1075,7 +1274,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="2"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1103,7 +1302,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="2"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1131,7 +1330,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="2"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1159,7 +1358,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1187,7 +1386,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="2"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -28370,10 +28569,6 @@
       <c r="Z1000" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A10:E10"/>
-  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished conversion of building cell data into data structures
</commit_message>
<xml_diff>
--- a/building_test.xlsx
+++ b/building_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="88">
   <si>
     <t>Room  121</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>Room  123</t>
+  </si>
+  <si>
+    <t>corridor</t>
   </si>
   <si>
     <t>hall</t>
@@ -61,6 +64,21 @@
     <t>Room  124</t>
   </si>
   <si>
+    <t>Room 169</t>
+  </si>
+  <si>
+    <t>Room 170</t>
+  </si>
+  <si>
+    <t>Room 171</t>
+  </si>
+  <si>
+    <t>Room 172</t>
+  </si>
+  <si>
+    <t>Room 173</t>
+  </si>
+  <si>
     <t>Room 106</t>
   </si>
   <si>
@@ -74,6 +92,21 @@
   </si>
   <si>
     <t>Room 110</t>
+  </si>
+  <si>
+    <t>Room 178</t>
+  </si>
+  <si>
+    <t>Room 177</t>
+  </si>
+  <si>
+    <t>Room 176</t>
+  </si>
+  <si>
+    <t>Room 175</t>
+  </si>
+  <si>
+    <t>Room 174</t>
   </si>
   <si>
     <t>Room 111</t>
@@ -91,6 +124,9 @@
     <t>Room 115</t>
   </si>
   <si>
+    <t>Room 179</t>
+  </si>
+  <si>
     <t>Room 116</t>
   </si>
   <si>
@@ -106,10 +142,31 @@
     <t>Room 120</t>
   </si>
   <si>
+    <t>Room 184</t>
+  </si>
+  <si>
+    <t>Room 183</t>
+  </si>
+  <si>
+    <t>Room 182</t>
+  </si>
+  <si>
+    <t>Room 181</t>
+  </si>
+  <si>
+    <t>Room 180</t>
+  </si>
+  <si>
     <t>Room 129</t>
   </si>
   <si>
     <t>Room 148</t>
+  </si>
+  <si>
+    <t>Room 149</t>
+  </si>
+  <si>
+    <t>Room 168</t>
   </si>
   <si>
     <t>Room 130</t>
@@ -118,10 +175,22 @@
     <t>Room 147</t>
   </si>
   <si>
+    <t>Room 150</t>
+  </si>
+  <si>
+    <t>Room 167</t>
+  </si>
+  <si>
     <t>Room 131</t>
   </si>
   <si>
     <t>Room 146</t>
+  </si>
+  <si>
+    <t>Room 151</t>
+  </si>
+  <si>
+    <t>Room 166</t>
   </si>
   <si>
     <t>Room 132</t>
@@ -130,10 +199,22 @@
     <t>Room 145</t>
   </si>
   <si>
+    <t>Room 152</t>
+  </si>
+  <si>
+    <t>Room 165</t>
+  </si>
+  <si>
     <t>Room 133</t>
   </si>
   <si>
     <t>Room 144</t>
+  </si>
+  <si>
+    <t>Room 153</t>
+  </si>
+  <si>
+    <t>Room 164</t>
   </si>
   <si>
     <t>Room 134</t>
@@ -142,10 +223,22 @@
     <t>Room 143</t>
   </si>
   <si>
+    <t>Room 154</t>
+  </si>
+  <si>
+    <t>Room 163</t>
+  </si>
+  <si>
     <t>Room 135</t>
   </si>
   <si>
     <t>Room 142</t>
+  </si>
+  <si>
+    <t>Room 155</t>
+  </si>
+  <si>
+    <t>Room 162</t>
   </si>
   <si>
     <t>Room 136</t>
@@ -154,16 +247,34 @@
     <t>Room 141</t>
   </si>
   <si>
+    <t>Room 156</t>
+  </si>
+  <si>
+    <t>Room 161</t>
+  </si>
+  <si>
     <t>Room 137</t>
   </si>
   <si>
     <t>Room 140</t>
   </si>
   <si>
+    <t>Room 157</t>
+  </si>
+  <si>
+    <t>Room 160</t>
+  </si>
+  <si>
     <t>Room 138</t>
   </si>
   <si>
     <t>Room 139</t>
+  </si>
+  <si>
+    <t>Room 158</t>
+  </si>
+  <si>
+    <t>Room 159</t>
   </si>
 </sst>
 </file>
@@ -518,23 +629,25 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="2"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -552,42 +665,54 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="K5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -600,32 +725,44 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -638,32 +775,44 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -680,13 +829,15 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -704,32 +855,46 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="L9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -742,32 +907,46 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
+      <c r="L10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -780,32 +959,56 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -822,13 +1025,25 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="J12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -851,18 +1066,24 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="J13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -885,18 +1106,24 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+      <c r="J14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -919,18 +1146,24 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+      <c r="J15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -953,18 +1186,24 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="J16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -987,18 +1226,24 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="J17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1021,18 +1266,24 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="J18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1055,18 +1306,24 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="J19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1089,18 +1346,24 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="J20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1123,18 +1386,24 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="J21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1156,15 +1425,6 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>

</xml_diff>

<commit_message>
Added room assignment between rooms and tenants
</commit_message>
<xml_diff>
--- a/building_test.xlsx
+++ b/building_test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
   <si>
     <t>Room  121</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Room  122</t>
   </si>
   <si>
-    <t>Room 123</t>
+    <t xml:space="preserve">Room 123 </t>
   </si>
   <si>
     <t>Room  123</t>
@@ -43,7 +43,7 @@
     <t>Room 103</t>
   </si>
   <si>
-    <t>Room 102</t>
+    <t>Room 102 | 2 beds</t>
   </si>
   <si>
     <t>Room 101</t>
@@ -67,7 +67,7 @@
     <t>Room 169</t>
   </si>
   <si>
-    <t>Room 170</t>
+    <t>Room 170 | 2 beds</t>
   </si>
   <si>
     <t>Room 171</t>
@@ -82,7 +82,7 @@
     <t>Room 106</t>
   </si>
   <si>
-    <t>Room 107</t>
+    <t>Room 107 | 2 beds</t>
   </si>
   <si>
     <t>Room 108</t>
@@ -103,7 +103,7 @@
     <t>Room 176</t>
   </si>
   <si>
-    <t>Room 175</t>
+    <t>Room 175 | 2 beds</t>
   </si>
   <si>
     <t>Room 174</t>
@@ -124,7 +124,10 @@
     <t>Room 115</t>
   </si>
   <si>
-    <t>Room 179</t>
+    <t>Room 175</t>
+  </si>
+  <si>
+    <t>Room 179 | 2 beds</t>
   </si>
   <si>
     <t>Room 116</t>
@@ -145,7 +148,7 @@
     <t>Room 184</t>
   </si>
   <si>
-    <t>Room 183</t>
+    <t>Room 183 | 2 beds</t>
   </si>
   <si>
     <t>Room 182</t>
@@ -647,7 +650,9 @@
       <c r="K4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -697,7 +702,9 @@
       <c r="K5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="M5" s="2" t="s">
         <v>17</v>
       </c>
@@ -747,7 +754,9 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="M6" s="2" t="s">
         <v>6</v>
       </c>
@@ -797,7 +806,9 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="M7" s="2" t="s">
         <v>27</v>
       </c>
@@ -837,7 +848,9 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -881,7 +894,7 @@
         <v>5</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>29</v>
@@ -893,7 +906,7 @@
         <v>27</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -959,19 +972,19 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
@@ -995,19 +1008,19 @@
         <v>5</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -1026,23 +1039,23 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -1066,23 +1079,23 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -1106,23 +1119,23 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -1146,23 +1159,23 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -1186,23 +1199,23 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -1226,23 +1239,23 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
@@ -1266,23 +1279,23 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1306,23 +1319,23 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1346,23 +1359,23 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1386,23 +1399,23 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>6</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>

</xml_diff>